<commit_message>
Finalized report for Act 2
</commit_message>
<xml_diff>
--- a/[1] Camera Calibration/Test vs Prediction.xlsx
+++ b/[1] Camera Calibration/Test vs Prediction.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upsystem-my.sharepoint.com/personal/ncramones_outlook_up_edu_ph/Documents/AY 2023-2024/First Semester/App Physics 167/[1] Camera Calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FB26998-6C4B-4410-9914-EF69E0864F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{3FB26998-6C4B-4410-9914-EF69E0864F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC18F8C3-D611-4FFA-9FC9-0EB851F63900}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{379521B7-8A5B-4F86-A05F-3A0F68E9EC70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <r>
       <t xml:space="preserve">Test </t>
@@ -97,12 +97,42 @@
       <t>yi</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Diff </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aileron Heavy"/>
+        <family val="3"/>
+      </rPr>
+      <t>x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Diff </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aileron Heavy"/>
+        <family val="3"/>
+      </rPr>
+      <t>y</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,19 +165,21 @@
       <name val="Aileron Heavy"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -173,12 +205,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114CCED0-D095-4187-8791-AC38AD299736}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,7 +540,7 @@
     <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,8 +553,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>248</v>
       </c>
@@ -534,8 +573,16 @@
       <c r="D2" s="1">
         <v>495</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <f>ABS(A2-C2)</f>
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <f>ABS(B2-D2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>153</v>
       </c>
@@ -548,8 +595,16 @@
       <c r="D3" s="1">
         <v>545</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <f t="shared" ref="E3:E21" si="0">ABS(A3-C3)</f>
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F21" si="1">ABS(B3-D3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>210</v>
       </c>
@@ -562,8 +617,16 @@
       <c r="D4" s="1">
         <v>467</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>188</v>
       </c>
@@ -576,8 +639,16 @@
       <c r="D5" s="1">
         <v>434</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>143</v>
       </c>
@@ -590,8 +661,16 @@
       <c r="D6" s="1">
         <v>456</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>244</v>
       </c>
@@ -604,8 +683,16 @@
       <c r="D7" s="1">
         <v>387</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>222</v>
       </c>
@@ -618,8 +705,16 @@
       <c r="D8" s="1">
         <v>325</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>149</v>
       </c>
@@ -632,8 +727,16 @@
       <c r="D9" s="1">
         <v>285</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>114</v>
       </c>
@@ -646,8 +749,16 @@
       <c r="D10" s="1">
         <v>442</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>130</v>
       </c>
@@ -660,8 +771,16 @@
       <c r="D11" s="1">
         <v>350</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>297</v>
       </c>
@@ -674,8 +793,16 @@
       <c r="D12" s="1">
         <v>493</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>377</v>
       </c>
@@ -688,8 +815,16 @@
       <c r="D13" s="1">
         <v>540</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>356</v>
       </c>
@@ -702,8 +837,16 @@
       <c r="D14" s="1">
         <v>506</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>316</v>
       </c>
@@ -716,8 +859,16 @@
       <c r="D15" s="1">
         <v>464</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>383</v>
       </c>
@@ -730,8 +881,16 @@
       <c r="D16" s="1">
         <v>450</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>339</v>
       </c>
@@ -744,8 +903,16 @@
       <c r="D17" s="1">
         <v>407</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>296</v>
       </c>
@@ -758,8 +925,16 @@
       <c r="D18" s="1">
         <v>370</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>297</v>
       </c>
@@ -772,8 +947,16 @@
       <c r="D19" s="1">
         <v>323</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>391</v>
       </c>
@@ -786,8 +969,16 @@
       <c r="D20" s="1">
         <v>343</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>278</v>
       </c>
@@ -799,6 +990,24 @@
       </c>
       <c r="D21" s="1">
         <v>342</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E22" s="6">
+        <f>AVERAGE(E2:E21)</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="6">
+        <f>AVERAGE(F2:F21)</f>
+        <v>1.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>